<commit_message>
work on autoclicker with selenium, somewhat finished, needs to be tested
</commit_message>
<xml_diff>
--- a/query/aurora_wos_v2.xlsx
+++ b/query/aurora_wos_v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="SDG1" sheetId="1" state="visible" r:id="rId2"/>
@@ -1580,10 +1580,10 @@
     <t xml:space="preserve">By 2020, ensure the conservation, restoration and sustainable use of terrestrial and inland freshwater ecosystems and their services, in particular forests, wetlands, mountains and drylands, in line with obligations under international agreements 15.1.1 Forest area as a proportion of total land area 15.1.2 Proportion of important sites for terrestrial and freshwater biodiversity that are covered by protected areas, by ecosystem type </t>
   </si>
   <si>
-    <t xml:space="preserve">TITLE-ABS-KEY ( ( ( "sustainab*" OR "conserv*" OR "restor*" ) W/3 ( "ecosyst*" OR "terrestrial" OR "freshwater" OR "inland" OR "forest*" OR "rainforest*" OR "agroforest*" OR "deforest*" OR "reforest*" OR "afforest*" OR "environment*" OR "soil" OR "land" ) ) AND NOT ( "marine" OR "ocean*" OR "sea" OR "seas" OR "reef" ) ) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TS = ( ( ( "sustainab*" OR "conserv*" OR "restor*" ) NEAR/3 ( "ecosyst*" OR "terrestrial" OR "freshwater" OR "inland" OR "forest*" OR "rainforest*" OR "agroforest*" OR "deforest*" OR "reforest*" OR "afforest*" OR "environment*" OR "soil" OR "land" ) ) AND NOT ( "marine" OR "ocean*" OR "sea" OR "seas" OR "reef" ) ) </t>
+    <t xml:space="preserve">TITLE-ABS-KEY ( ( ( "sustainab*" OR "conserv*" OR "restor*" ) W/3 ( "ecosyst*" OR "terrestrial" OR "freshwater" OR "inland" OR "forest*" OR "rainforest*" OR "agroforest*" OR "deforest*" OR "reforest*" OR "afforest*" OR "environment*" OR "soil" OR "land" ) ) NOT ( "marine" OR "ocean*" OR "sea" OR "seas" OR "reef" ) ) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TS = ( ( ( "sustainab*" OR "conserv*" OR "restor*" ) NEAR/3 ( "ecosyst*" OR "terrestrial" OR "freshwater" OR "inland" OR "forest*" OR "rainforest*" OR "agroforest*" OR "deforest*" OR "reforest*" OR "afforest*" OR "environment*" OR "soil" OR "land" ) ) NOT ( "marine" OR "ocean*" OR "sea" OR "seas" OR "reef" ) ) </t>
   </si>
   <si>
     <t xml:space="preserve">15. 2</t>
@@ -1652,10 +1652,10 @@
     <t xml:space="preserve">Take urgent action to end poaching and trafficking of protected species of flora and fauna and address both demand and supply of illegal wildlife products 15.7.1 Proportion of traded wildlife that was poached or illicitly trafficked </t>
   </si>
   <si>
-    <t xml:space="preserve">OR TITLE-ABS-KEY ( ( "poaching" OR "trafficking") AND ("species" OR "flora" OR "fauna" OR "wildlife") AND NOT ("marine" OR "ocean*" OR "sea" OR "seas" OR "reef") ) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TS = ( ( "poaching" OR "trafficking") AND ("species" OR "flora" OR "fauna" OR "wildlife") AND NOT ("marine" OR "ocean*" OR "sea" OR "seas" OR "reef") ) </t>
+    <t xml:space="preserve">OR TITLE-ABS-KEY ( ( "poaching" OR "trafficking") AND ("species" OR "flora" OR "fauna" OR "wildlife") NOT ("marine" OR "ocean*" OR "sea" OR "seas" OR "reef") ) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TS = ( ( "poaching" OR "trafficking") AND ("species" OR "flora" OR "fauna" OR "wildlife") NOT ("marine" OR "ocean*" OR "sea" OR "seas" OR "reef") ) </t>
   </si>
   <si>
     <t xml:space="preserve">15. 8</t>
@@ -1664,10 +1664,10 @@
     <t xml:space="preserve">By 2020, introduce measures to prevent the introduction and significantly reduce the impact of invasive alien species on land and water ecosystems and control or eradicate the priority species 15.8.1 Proportion of countries adopting relevant national legislation and adequately resourcing the prevention or control of invasive alien species </t>
   </si>
   <si>
-    <t xml:space="preserve">OR TITLE-ABS-KEY ( ( "invas*" ) W/3 ( "alien" OR "nonnative" OR "non-native" OR "nonindigenous" OR "non-indigenous" ) W/3 ( "species" OR "animal*" OR "plant*" ) AND NOT ("marine" OR "ocean*" OR "sea" OR "seas" OR "reef") ) OR TITLE-ABS-KEY ( ( "protect*" ) W/3 ( "threaten*" OR "endanger*" ) W/3 ( "species" OR "animal*" OR "plant*" ) AND NOT ("marine" OR "ocean*" OR "sea" OR "seas" OR "reef") ) OR TITLE-ABS-KEY ( ( ( "prevent*" ) W/3 ( "extinct*" ) ) AND ( ( "threaten*" OR "endanger*" ) W/3 ( "species" OR "animal*" OR "plant*" ) ) AND NOT ("marine" OR "ocean*" OR "sea" OR "seas" OR "reef") ) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TS = ( ( "invas*" ) NEAR/3 ( "alien" OR "nonnative" OR "non-native" OR "nonindigenous" OR "non-indigenous" ) NEAR/3 ( "species" OR "animal*" OR "plant*" ) AND NOT ("marine" OR "ocean*" OR "sea" OR "seas" OR "reef") ) OR TS = ( ( "protect*" ) NEAR/3 ( "threaten*" OR "endanger*" ) NEAR/3 ( "species" OR "animal*" OR "plant*" ) AND NOT ("marine" OR "ocean*" OR "sea" OR "seas" OR "reef") ) OR TS = ( ( ( "prevent*" ) NEAR/3 ( "extinct*" ) ) AND ( ( "threaten*" OR "endanger*" ) NEAR/3 ( "species" OR "animal*" OR "plant*" ) ) AND NOT ("marine" OR "ocean*" OR "sea" OR "seas" OR "reef") ) </t>
+    <t xml:space="preserve">OR TITLE-ABS-KEY ( ( "invas*" ) W/3 ( "alien" OR "nonnative" OR "non-native" OR "nonindigenous" OR "non-indigenous" ) W/3 ( "species" OR "animal*" OR "plant*" ) NOT ("marine" OR "ocean*" OR "sea" OR "seas" OR "reef") ) OR TITLE-ABS-KEY ( ( "protect*" ) W/3 ( "threaten*" OR "endanger*" ) W/3 ( "species" OR "animal*" OR "plant*" ) NOT ("marine" OR "ocean*" OR "sea" OR "seas" OR "reef") ) OR TITLE-ABS-KEY ( ( ( "prevent*" ) W/3 ( "extinct*" ) ) AND ( ( "threaten*" OR "endanger*" ) W/3 ( "species" OR "animal*" OR "plant*" ) ) NOT ("marine" OR "ocean*" OR "sea" OR "seas" OR "reef") ) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TS = ( ( "invas*" ) NEAR/3 ( "alien" OR "nonnative" OR "non-native" OR "nonindigenous" OR "non-indigenous" ) NEAR/3 ( "species" OR "animal*" OR "plant*" ) NOT ("marine" OR "ocean*" OR "sea" OR "seas" OR "reef") ) OR TS = ( ( "protect*" ) NEAR/3 ( "threaten*" OR "endanger*" ) NEAR/3 ( "species" OR "animal*" OR "plant*" ) NOT ("marine" OR "ocean*" OR "sea" OR "seas" OR "reef") ) OR TS = ( ( ( "prevent*" ) NEAR/3 ( "extinct*" ) ) AND ( ( "threaten*" OR "endanger*" ) NEAR/3 ( "species" OR "animal*" OR "plant*" ) ) NOT ("marine" OR "ocean*" OR "sea" OR "seas" OR "reef") ) </t>
   </si>
   <si>
     <t xml:space="preserve">15. 9</t>
@@ -1676,10 +1676,10 @@
     <t xml:space="preserve">By 2020, integrate ecosystem and biodiversity values into national and local planning, development processes, poverty reduction strategies and accounts 15.9.1 Progress towards national targets established in accordance with Aichi Biodiversity Target 2 of the Strategic Plan for Biodiversity 2011-2020 </t>
   </si>
   <si>
-    <t xml:space="preserve">OR TITLE-ABS-KEY ( ( ( "ecosystem" W/3 "biodiversity" ) OR "species diversity" ) AND ( "polic*" OR "strateg*" OR "plan" OR "plans" OR "planning" ) AND NOT ("marine" OR "ocean*" OR "sea" OR "seas" OR "reef") ) OR TITLE-ABS-KEY ( ( "Aichi Biodiversity Target*" ) OR ( "Strategic Plan for Biodiversity" ) ) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TS = ( ( ( "ecosystem" NEAR/3 "biodiversity" ) OR "species diversity" ) AND ( "polic*" OR "strateg*" OR "plan" OR "plans" OR "planning" ) AND NOT ("marine" OR "ocean*" OR "sea" OR "seas" OR "reef") ) OR TS = ( ( "Aichi Biodiversity Target*" ) OR ( "Strategic Plan for Biodiversity" ) ) </t>
+    <t xml:space="preserve">OR TITLE-ABS-KEY ( ( ( "ecosystem" W/3 "biodiversity" ) OR "species diversity" ) AND ( "polic*" OR "strateg*" OR "plan" OR "plans" OR "planning" ) NOT ("marine" OR "ocean*" OR "sea" OR "seas" OR "reef") ) OR TITLE-ABS-KEY ( ( "Aichi Biodiversity Target*" ) OR ( "Strategic Plan for Biodiversity" ) ) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TS = ( ( ( "ecosystem" NEAR/3 "biodiversity" ) OR "species diversity" ) AND ( "polic*" OR "strateg*" OR "plan" OR "plans" OR "planning" ) NOT ("marine" OR "ocean*" OR "sea" OR "seas" OR "reef") ) OR TS = ( ( "Aichi Biodiversity Target*" ) OR ( "Strategic Plan for Biodiversity" ) ) </t>
   </si>
   <si>
     <t xml:space="preserve">15. a</t>
@@ -2171,13 +2171,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2193,7 +2197,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2203,7 +2207,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -2223,10 +2227,10 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2234,16 +2238,16 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2251,16 +2255,16 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2268,16 +2272,16 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2285,16 +2289,16 @@
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2302,16 +2306,16 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2319,16 +2323,16 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2336,16 +2340,16 @@
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2361,7 +2365,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2371,7 +2375,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -2391,10 +2395,10 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2402,16 +2406,16 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>328</v>
       </c>
     </row>
@@ -2419,16 +2423,16 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="2" t="s">
         <v>332</v>
       </c>
     </row>
@@ -2436,16 +2440,16 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="2" t="s">
         <v>336</v>
       </c>
     </row>
@@ -2453,16 +2457,16 @@
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="2" t="s">
         <v>340</v>
       </c>
     </row>
@@ -2470,16 +2474,16 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="2" t="s">
         <v>344</v>
       </c>
     </row>
@@ -2487,16 +2491,16 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="2" t="s">
         <v>348</v>
       </c>
     </row>
@@ -2504,16 +2508,16 @@
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="2" t="s">
         <v>352</v>
       </c>
     </row>
@@ -2521,16 +2525,16 @@
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="2" t="s">
         <v>356</v>
       </c>
     </row>
@@ -2538,16 +2542,16 @@
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="2" t="s">
         <v>360</v>
       </c>
     </row>
@@ -2555,16 +2559,16 @@
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="2" t="s">
         <v>364</v>
       </c>
     </row>
@@ -2580,7 +2584,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2590,7 +2594,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -2610,10 +2614,10 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2621,16 +2625,16 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>368</v>
       </c>
     </row>
@@ -2638,16 +2642,16 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="2" t="s">
         <v>372</v>
       </c>
     </row>
@@ -2655,16 +2659,16 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="2" t="s">
         <v>376</v>
       </c>
     </row>
@@ -2672,16 +2676,16 @@
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="2" t="s">
         <v>380</v>
       </c>
     </row>
@@ -2689,16 +2693,16 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="2" t="s">
         <v>384</v>
       </c>
     </row>
@@ -2706,16 +2710,16 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="2" t="s">
         <v>388</v>
       </c>
     </row>
@@ -2723,16 +2727,16 @@
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="2" t="s">
         <v>392</v>
       </c>
     </row>
@@ -2740,16 +2744,16 @@
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="2" t="s">
         <v>396</v>
       </c>
     </row>
@@ -2757,16 +2761,16 @@
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="2" t="s">
         <v>400</v>
       </c>
     </row>
@@ -2774,16 +2778,16 @@
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="2" t="s">
         <v>404</v>
       </c>
     </row>
@@ -2799,7 +2803,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2809,7 +2813,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -2829,10 +2833,10 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2840,16 +2844,16 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>408</v>
       </c>
     </row>
@@ -2857,16 +2861,16 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="2" t="s">
         <v>412</v>
       </c>
     </row>
@@ -2874,16 +2878,16 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="2" t="s">
         <v>416</v>
       </c>
     </row>
@@ -2891,16 +2895,16 @@
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="2" t="s">
         <v>420</v>
       </c>
     </row>
@@ -2908,16 +2912,16 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="2" t="s">
         <v>424</v>
       </c>
     </row>
@@ -2925,16 +2929,16 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="2" t="s">
         <v>428</v>
       </c>
     </row>
@@ -2942,16 +2946,16 @@
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="2" t="s">
         <v>432</v>
       </c>
     </row>
@@ -2959,16 +2963,16 @@
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="2" t="s">
         <v>436</v>
       </c>
     </row>
@@ -2976,16 +2980,16 @@
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="2" t="s">
         <v>440</v>
       </c>
     </row>
@@ -2993,16 +2997,16 @@
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="2" t="s">
         <v>443</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="2" t="s">
         <v>444</v>
       </c>
     </row>
@@ -3010,16 +3014,16 @@
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" s="2" t="s">
         <v>448</v>
       </c>
     </row>
@@ -3035,7 +3039,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3045,7 +3049,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -3065,10 +3069,10 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3076,13 +3080,13 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>451</v>
       </c>
     </row>
@@ -3090,16 +3094,16 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="2" t="s">
         <v>455</v>
       </c>
     </row>
@@ -3107,16 +3111,16 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="2" t="s">
         <v>459</v>
       </c>
     </row>
@@ -3124,16 +3128,16 @@
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="2" t="s">
         <v>463</v>
       </c>
     </row>
@@ -3141,16 +3145,16 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="2" t="s">
         <v>467</v>
       </c>
     </row>
@@ -3158,16 +3162,16 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="2" t="s">
         <v>469</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="2" t="s">
         <v>471</v>
       </c>
     </row>
@@ -3183,7 +3187,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3193,7 +3197,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -3213,10 +3217,10 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3224,16 +3228,16 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>475</v>
       </c>
     </row>
@@ -3241,16 +3245,16 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>477</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="2" t="s">
         <v>479</v>
       </c>
     </row>
@@ -3258,16 +3262,16 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="2" t="s">
         <v>483</v>
       </c>
     </row>
@@ -3275,16 +3279,16 @@
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="2" t="s">
         <v>486</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="2" t="s">
         <v>487</v>
       </c>
     </row>
@@ -3292,16 +3296,16 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="2" t="s">
         <v>491</v>
       </c>
     </row>
@@ -3309,16 +3313,16 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="2" t="s">
         <v>495</v>
       </c>
     </row>
@@ -3326,16 +3330,16 @@
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>496</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="2" t="s">
         <v>499</v>
       </c>
     </row>
@@ -3343,16 +3347,16 @@
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="2" t="s">
         <v>503</v>
       </c>
     </row>
@@ -3360,16 +3364,16 @@
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="2" t="s">
         <v>507</v>
       </c>
     </row>
@@ -3377,16 +3381,16 @@
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="2" t="s">
         <v>511</v>
       </c>
     </row>
@@ -3402,17 +3406,17 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J51" activeCellId="0" sqref="J51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -3432,10 +3436,10 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3443,16 +3447,16 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>513</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>514</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>515</v>
       </c>
     </row>
@@ -3460,16 +3464,16 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="2" t="s">
         <v>519</v>
       </c>
     </row>
@@ -3477,16 +3481,16 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="2" t="s">
         <v>523</v>
       </c>
     </row>
@@ -3494,16 +3498,16 @@
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="2" t="s">
         <v>526</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="2" t="s">
         <v>527</v>
       </c>
     </row>
@@ -3511,16 +3515,16 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="2" t="s">
         <v>531</v>
       </c>
     </row>
@@ -3528,16 +3532,16 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="2" t="s">
         <v>534</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="2" t="s">
         <v>535</v>
       </c>
     </row>
@@ -3545,16 +3549,16 @@
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="2" t="s">
         <v>539</v>
       </c>
     </row>
@@ -3562,16 +3566,16 @@
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="2" t="s">
         <v>541</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="2" t="s">
         <v>543</v>
       </c>
     </row>
@@ -3579,16 +3583,16 @@
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="2" t="s">
         <v>547</v>
       </c>
     </row>
@@ -3596,16 +3600,16 @@
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="2" t="s">
         <v>548</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="2" t="s">
         <v>551</v>
       </c>
     </row>
@@ -3613,16 +3617,16 @@
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" s="2" t="s">
         <v>555</v>
       </c>
     </row>
@@ -3630,16 +3634,16 @@
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" s="2" t="s">
         <v>539</v>
       </c>
     </row>
@@ -3655,7 +3659,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3665,7 +3669,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -3685,10 +3689,10 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3696,16 +3700,16 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>561</v>
       </c>
     </row>
@@ -3713,16 +3717,16 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>562</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>563</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>564</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="2" t="s">
         <v>565</v>
       </c>
     </row>
@@ -3730,16 +3734,16 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>566</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>567</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="2" t="s">
         <v>568</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="2" t="s">
         <v>569</v>
       </c>
     </row>
@@ -3747,16 +3751,16 @@
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="2" t="s">
         <v>571</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="2" t="s">
         <v>573</v>
       </c>
     </row>
@@ -3764,16 +3768,16 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>574</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="2" t="s">
         <v>576</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="2" t="s">
         <v>577</v>
       </c>
     </row>
@@ -3781,16 +3785,16 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>578</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="2" t="s">
         <v>579</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="2" t="s">
         <v>580</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="2" t="s">
         <v>581</v>
       </c>
     </row>
@@ -3798,16 +3802,16 @@
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>582</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="2" t="s">
         <v>583</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="2" t="s">
         <v>584</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="2" t="s">
         <v>585</v>
       </c>
     </row>
@@ -3815,16 +3819,16 @@
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="2" t="s">
         <v>587</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="2" t="s">
         <v>588</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="2" t="s">
         <v>589</v>
       </c>
     </row>
@@ -3832,16 +3836,16 @@
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="2" t="s">
         <v>590</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="2" t="s">
         <v>591</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="2" t="s">
         <v>592</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="2" t="s">
         <v>593</v>
       </c>
     </row>
@@ -3849,16 +3853,16 @@
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="2" t="s">
         <v>594</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="2" t="s">
         <v>595</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="2" t="s">
         <v>596</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="2" t="s">
         <v>597</v>
       </c>
     </row>
@@ -3866,16 +3870,16 @@
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="2" t="s">
         <v>598</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="2" t="s">
         <v>599</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="2" t="s">
         <v>600</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" s="2" t="s">
         <v>601</v>
       </c>
     </row>
@@ -3883,16 +3887,16 @@
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="2" t="s">
         <v>602</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="2" t="s">
         <v>603</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="2" t="s">
         <v>604</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" s="2" t="s">
         <v>605</v>
       </c>
     </row>
@@ -3908,7 +3912,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3918,7 +3922,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -3938,10 +3942,10 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3949,16 +3953,16 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>606</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>607</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>608</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>609</v>
       </c>
     </row>
@@ -3966,16 +3970,16 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>610</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>611</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>612</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="2" t="s">
         <v>613</v>
       </c>
     </row>
@@ -3983,16 +3987,16 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>614</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>615</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="2" t="s">
         <v>616</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="2" t="s">
         <v>617</v>
       </c>
     </row>
@@ -4000,16 +4004,16 @@
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>618</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="2" t="s">
         <v>619</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="2" t="s">
         <v>621</v>
       </c>
     </row>
@@ -4017,16 +4021,16 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>622</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>623</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="2" t="s">
         <v>624</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="2" t="s">
         <v>625</v>
       </c>
     </row>
@@ -4034,16 +4038,16 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>626</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="2" t="s">
         <v>628</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="2" t="s">
         <v>629</v>
       </c>
     </row>
@@ -4051,16 +4055,16 @@
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>630</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="2" t="s">
         <v>631</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="2" t="s">
         <v>632</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="2" t="s">
         <v>633</v>
       </c>
     </row>
@@ -4068,16 +4072,16 @@
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>634</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="2" t="s">
         <v>635</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="2" t="s">
         <v>636</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="2" t="s">
         <v>637</v>
       </c>
     </row>
@@ -4085,16 +4089,16 @@
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="2" t="s">
         <v>638</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="2" t="s">
         <v>639</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="2" t="s">
         <v>640</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="2" t="s">
         <v>641</v>
       </c>
     </row>
@@ -4102,16 +4106,16 @@
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="2" t="s">
         <v>642</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="2" t="s">
         <v>643</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="2" t="s">
         <v>644</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="2" t="s">
         <v>645</v>
       </c>
     </row>
@@ -4119,16 +4123,16 @@
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="2" t="s">
         <v>646</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="2" t="s">
         <v>647</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="2" t="s">
         <v>648</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" s="2" t="s">
         <v>649</v>
       </c>
     </row>
@@ -4136,16 +4140,16 @@
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="2" t="s">
         <v>650</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="2" t="s">
         <v>651</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="2" t="s">
         <v>652</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" s="2" t="s">
         <v>653</v>
       </c>
     </row>
@@ -4153,16 +4157,16 @@
       <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="2" t="s">
         <v>654</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="2" t="s">
         <v>655</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="2" t="s">
         <v>656</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" s="2" t="s">
         <v>657</v>
       </c>
     </row>
@@ -4170,16 +4174,16 @@
       <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="2" t="s">
         <v>658</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="2" t="s">
         <v>659</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="2" t="s">
         <v>660</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="E16" s="2" t="s">
         <v>661</v>
       </c>
     </row>
@@ -4187,16 +4191,16 @@
       <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="2" t="s">
         <v>662</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="2" t="s">
         <v>663</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="2" t="s">
         <v>664</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="E17" s="2" t="s">
         <v>665</v>
       </c>
     </row>
@@ -4204,16 +4208,16 @@
       <c r="A18" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="2" t="s">
         <v>666</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="2" t="s">
         <v>667</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="2" t="s">
         <v>668</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="E18" s="2" t="s">
         <v>669</v>
       </c>
     </row>
@@ -4221,16 +4225,16 @@
       <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="2" t="s">
         <v>670</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="2" t="s">
         <v>671</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="E19" s="2" t="s">
         <v>673</v>
       </c>
     </row>
@@ -4238,16 +4242,16 @@
       <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="2" t="s">
         <v>674</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="2" t="s">
         <v>675</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="2" t="s">
         <v>676</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="E20" s="2" t="s">
         <v>677</v>
       </c>
     </row>
@@ -4255,16 +4259,16 @@
       <c r="A21" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="2" t="s">
         <v>678</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="2" t="s">
         <v>679</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="2" t="s">
         <v>680</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="E21" s="2" t="s">
         <v>681</v>
       </c>
     </row>
@@ -4280,7 +4284,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -4290,7 +4294,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -4310,10 +4314,10 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4321,16 +4325,16 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4338,16 +4342,16 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="2" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4355,16 +4359,16 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="2" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4372,16 +4376,16 @@
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="2" t="s">
         <v>48</v>
       </c>
     </row>
@@ -4389,16 +4393,16 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="2" t="s">
         <v>52</v>
       </c>
     </row>
@@ -4406,16 +4410,16 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="2" t="s">
         <v>56</v>
       </c>
     </row>
@@ -4423,16 +4427,16 @@
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="2" t="s">
         <v>60</v>
       </c>
     </row>
@@ -4440,16 +4444,16 @@
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="2" t="s">
         <v>64</v>
       </c>
     </row>
@@ -4465,17 +4469,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -4495,10 +4499,10 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4506,16 +4510,16 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>68</v>
       </c>
     </row>
@@ -4523,16 +4527,16 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="2" t="s">
         <v>72</v>
       </c>
     </row>
@@ -4540,16 +4544,16 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="2" t="s">
         <v>76</v>
       </c>
     </row>
@@ -4557,16 +4561,16 @@
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="2" t="s">
         <v>80</v>
       </c>
     </row>
@@ -4574,16 +4578,16 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="2" t="s">
         <v>84</v>
       </c>
     </row>
@@ -4591,16 +4595,16 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="2" t="s">
         <v>88</v>
       </c>
     </row>
@@ -4608,16 +4612,16 @@
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="2" t="s">
         <v>92</v>
       </c>
     </row>
@@ -4625,16 +4629,16 @@
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="2" t="s">
         <v>96</v>
       </c>
     </row>
@@ -4642,16 +4646,16 @@
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="2" t="s">
         <v>100</v>
       </c>
     </row>
@@ -4659,16 +4663,16 @@
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="2" t="s">
         <v>104</v>
       </c>
     </row>
@@ -4676,16 +4680,16 @@
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" s="2" t="s">
         <v>108</v>
       </c>
     </row>
@@ -4693,16 +4697,16 @@
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" s="2" t="s">
         <v>112</v>
       </c>
     </row>
@@ -4710,16 +4714,16 @@
       <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" s="2" t="s">
         <v>116</v>
       </c>
     </row>
@@ -4735,7 +4739,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -4745,7 +4749,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -4765,10 +4769,10 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4776,16 +4780,16 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>120</v>
       </c>
     </row>
@@ -4793,16 +4797,16 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="2" t="s">
         <v>124</v>
       </c>
     </row>
@@ -4810,16 +4814,16 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="2" t="s">
         <v>128</v>
       </c>
     </row>
@@ -4827,16 +4831,16 @@
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="2" t="s">
         <v>132</v>
       </c>
     </row>
@@ -4844,16 +4848,16 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="2" t="s">
         <v>136</v>
       </c>
     </row>
@@ -4861,16 +4865,16 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="2" t="s">
         <v>140</v>
       </c>
     </row>
@@ -4878,16 +4882,16 @@
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="2" t="s">
         <v>144</v>
       </c>
     </row>
@@ -4895,16 +4899,16 @@
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="2" t="s">
         <v>148</v>
       </c>
     </row>
@@ -4912,16 +4916,16 @@
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="2" t="s">
         <v>152</v>
       </c>
     </row>
@@ -4929,16 +4933,16 @@
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="2" t="s">
         <v>156</v>
       </c>
     </row>
@@ -4954,7 +4958,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -4964,7 +4968,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -4984,10 +4988,10 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4995,16 +4999,16 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>160</v>
       </c>
     </row>
@@ -5012,16 +5016,16 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="2" t="s">
         <v>164</v>
       </c>
     </row>
@@ -5029,16 +5033,16 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="2" t="s">
         <v>168</v>
       </c>
     </row>
@@ -5046,16 +5050,16 @@
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="2" t="s">
         <v>172</v>
       </c>
     </row>
@@ -5063,16 +5067,16 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="2" t="s">
         <v>176</v>
       </c>
     </row>
@@ -5080,16 +5084,16 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5097,16 +5101,16 @@
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="2" t="s">
         <v>184</v>
       </c>
     </row>
@@ -5114,16 +5118,16 @@
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="2" t="s">
         <v>188</v>
       </c>
     </row>
@@ -5131,16 +5135,16 @@
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="2" t="s">
         <v>192</v>
       </c>
     </row>
@@ -5156,7 +5160,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -5166,7 +5170,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -5186,10 +5190,10 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5197,16 +5201,16 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>196</v>
       </c>
     </row>
@@ -5214,16 +5218,16 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="2" t="s">
         <v>200</v>
       </c>
     </row>
@@ -5231,16 +5235,16 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="2" t="s">
         <v>204</v>
       </c>
     </row>
@@ -5248,16 +5252,16 @@
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="2" t="s">
         <v>208</v>
       </c>
     </row>
@@ -5265,16 +5269,16 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="2" t="s">
         <v>212</v>
       </c>
     </row>
@@ -5282,16 +5286,16 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="2" t="s">
         <v>216</v>
       </c>
     </row>
@@ -5299,16 +5303,16 @@
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="2" t="s">
         <v>220</v>
       </c>
     </row>
@@ -5316,16 +5320,16 @@
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="2" t="s">
         <v>224</v>
       </c>
     </row>
@@ -5341,7 +5345,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -5351,7 +5355,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -5371,10 +5375,10 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5382,16 +5386,16 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>228</v>
       </c>
     </row>
@@ -5399,16 +5403,16 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="2" t="s">
         <v>232</v>
       </c>
     </row>
@@ -5416,16 +5420,16 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="2" t="s">
         <v>236</v>
       </c>
     </row>
@@ -5433,16 +5437,16 @@
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="2" t="s">
         <v>240</v>
       </c>
     </row>
@@ -5450,16 +5454,16 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="2" t="s">
         <v>244</v>
       </c>
     </row>
@@ -5475,7 +5479,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -5485,7 +5489,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -5505,10 +5509,10 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5516,16 +5520,16 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>248</v>
       </c>
     </row>
@@ -5533,16 +5537,16 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="2" t="s">
         <v>252</v>
       </c>
     </row>
@@ -5550,16 +5554,16 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="2" t="s">
         <v>256</v>
       </c>
     </row>
@@ -5567,16 +5571,16 @@
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="2" t="s">
         <v>260</v>
       </c>
     </row>
@@ -5584,16 +5588,16 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="2" t="s">
         <v>264</v>
       </c>
     </row>
@@ -5601,16 +5605,16 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="2" t="s">
         <v>268</v>
       </c>
     </row>
@@ -5618,16 +5622,16 @@
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="2" t="s">
         <v>272</v>
       </c>
     </row>
@@ -5635,16 +5639,16 @@
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="2" t="s">
         <v>276</v>
       </c>
     </row>
@@ -5652,16 +5656,16 @@
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="2" t="s">
         <v>280</v>
       </c>
     </row>
@@ -5669,16 +5673,16 @@
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="2" t="s">
         <v>284</v>
       </c>
     </row>
@@ -5686,16 +5690,16 @@
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" s="2" t="s">
         <v>288</v>
       </c>
     </row>
@@ -5703,16 +5707,16 @@
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" s="2" t="s">
         <v>292</v>
       </c>
     </row>
@@ -5728,7 +5732,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -5738,7 +5742,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -5758,10 +5762,10 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5769,16 +5773,16 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>296</v>
       </c>
     </row>
@@ -5786,16 +5790,16 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="2" t="s">
         <v>300</v>
       </c>
     </row>
@@ -5803,16 +5807,16 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="2" t="s">
         <v>304</v>
       </c>
     </row>
@@ -5820,16 +5824,16 @@
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="2" t="s">
         <v>308</v>
       </c>
     </row>
@@ -5837,16 +5841,16 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="2" t="s">
         <v>312</v>
       </c>
     </row>
@@ -5854,16 +5858,16 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="2" t="s">
         <v>316</v>
       </c>
     </row>
@@ -5871,16 +5875,16 @@
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="2" t="s">
         <v>320</v>
       </c>
     </row>
@@ -5888,16 +5892,16 @@
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="2" t="s">
         <v>324</v>
       </c>
     </row>

</xml_diff>